<commit_message>
Nisja e krijimit te statistika aplikimesh
</commit_message>
<xml_diff>
--- a/ExcelFiles/Statusi Sherbimit.xlsx
+++ b/ExcelFiles/Statusi Sherbimit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arbi.topi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arbi.topi\IdeaProjects\TestimTemp\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43A8FBF-E717-4EA9-9941-8929E4684481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28664468-7B26-4B7D-AE0B-3EC774B802F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9495" yWindow="-18270" windowWidth="23040" windowHeight="8970" xr2:uid="{AF40D6F3-C384-4093-AD10-2C6B76FDF766}"/>
+    <workbookView xWindow="10020" yWindow="-17055" windowWidth="23040" windowHeight="8970" xr2:uid="{AF40D6F3-C384-4093-AD10-2C6B76FDF766}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>